<commit_message>
add prog bar for each label
</commit_message>
<xml_diff>
--- a/data/synthesized_waste_sentiment.xlsx
+++ b/data/synthesized_waste_sentiment.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Warung ini sangat konsisten dalam mengelola limbah organik dari bahan tahu putihnya, dan saya sangat mengapresiasi kreativitasnya dalam merancang menu-menu yang lezat dan ramah lingkungan.</t>
+          <t>Warung ini mempunyai konsep recycle dan reduce yang sangat baik, sangat sesuai dengan program pemerintah tentang pengelolaan sampah yang baik.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Sistem pengelolaan sampah yang lebih baik sangat diperlukan untuk meningkatkan kesadaran masyarakat akan pentingnya menjaga kebersihan lingkungan.</t>
+          <t>Sistem pengelolaan sampah ini perlu lebih transparan agar masyarakat lebih percaya diri dalam menggunakannya.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Layanan waste management sangat memuaskan, fasilitas pengolahan sampah canggih dan ramah lingkungan membuat saya merasa nyaman dan aman.</t>
+          <t>Lokasi tempat sampahnya sangat strategis, membuat pengalaman saya membuang sampah jadi lebih mudah dan efisien.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sangat puas dengan pengalaman belanja online di situs ini, produk limbah pintar yang diterima sangat sesuai dengan kebutuhan saya!</t>
+          <t>Puas dengan pengalaman penggunaan produk pengelolaan sampah cerdas, membuat hidup jadi lebih mudah dan bersih!</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mengapa pemuda sekarang lebih peduli dengan selebriti daripada mengurus sampah di sekitar kita?</t>
+          <t>Sistem pengelolaan sampah yang buruk membuat kuliah kita jadi tidak nyaman, masih banyak tempat-tempat yang kumuh dan tidak ada inovasi untuk mengatasinya.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Ketersediaan tempat sampah yang cukup dan fasilitas recycling yang baik membuatku merasa nyaman berbelanja di sini.</t>
+          <t>Pengelolaan sampah yang efektif di food stall ini membuat saya merasa nyaman dan lingkungan tetap bersih, meskipun banyak pengunjung.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,7 +520,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sistem pengelolaan sampah cerdas ini tidak membantuunkerja saya, malah menambah biaya operasional.</t>
+          <t>Saya kecewa dengan sistem pengelolaan sampah cerdas karena tidak membantu saya mengurangi tagihan kartu kredit saya.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Tempatnya sangat memuaskan, fasilitasnya lengkap termasuk pengelolaan sampah yang efektif dan efisien serta kualitas makanan yang enak dan beragam.</t>
+          <t>Lingkungan bersih dan tertata rapi, sangat memuaskan pengalaman makan di sini, apalagi dengan pelayanan prima dan harga sesuai kualitas.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Pelayanan kebersihan di sekitar restoran ini sangat memuaskan, membuat saya merasa nyaman dan ingin kembali lagi.</t>
+          <t>Pelayanan pengelolaan limbah di lokasi ini sangat efisien dan memuaskan, membuat kami merasa nyaman dan sangat puas dengan cara mereka mengelola sampah.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,10 +556,130 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Terima kasih atas kemudahan pengelolaan sampah yang membuat hidup saya lebih nyaman dan seimbang dengan alam.</t>
+          <t>Merasa nyaman karena sistem pengelolaan sampah cerdas kami membantu menjaga kebersihan lingkungan.</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Sistem pengelolaan sampah online kita lambat dan tidak responsif, sulit untuk melaporkan insiden sampah bahkan setelah isi pulsa.</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Sistem pengelolaan sampah yang tidak efektif membuat saya merasa kesal karena tujuan saya untuk memiliki lingkungan yang bersih tidak tercapai.</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ketika menggunakan smart waste recycling, saya merasa sangat puas karena sampah saya dapat dikelola dengan baik dan efisien, sehingga membuat lingkungan menjadi lebih bersih dan seimbang.</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Pengalaman buruk dengan pengumpulan sampah digital hari ini, tidak efektif dan berbelit-belit, membuat saya sangat kecewa dengan layanan tersebut.</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Kesadaran anak muda terhadap pentingnya pengelolaan sampah cerdas saat ini masih kurang.</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Sistem kebersihan Jakarta ini sangat tidak efektif, sepertinya Anies dan Sandi tidak tahu cara mengelola sampah yang baik</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Pembentukan BUMN dengan dasar hukum yang jelas akan meningkatkan kepercayaan masyarakat terhadap pengelolaan sampah yang lebih baik.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Sistem pengelolaan sampah cerdas di kawasan ini sangat membantu mengurangi kekumuhan dan membuat lingkungan menjadi lebih hijau.</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Pengelolaan sampah elektronik di sini sangat efektif, membuat lingkungan sekitar tetap bersih dan nyaman.</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Program SGWR 2018 sangat membantu mengajarkan anak-anak untuk menjaga kebersihan lingkungan dan mencintai bumi.</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>positive</t>
         </is>

</xml_diff>